<commit_message>
Skip specific columns for POINT geo type in export for (T11) form
Added logic to exclude 't_ctry', 't_site_name', and 't_noise_temp' columns when processing rows with geo type 'POINT' in the Excel to text conversion. This ensures only relevant data is exported for each geo type.
</commit_message>
<xml_diff>
--- a/Data Dummy/Test Excel.xlsx
+++ b/Data Dummy/Test Excel.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\e-notice-Converter\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/87c52a275ae1046c/Work/Ongoing/e-notice/Convert App ^0 Template Form/Convert e-notice/Data Dummy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE47BB07-B845-4614-97BD-04492A22F008}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="13_ncr:1_{AE47BB07-B845-4614-97BD-04492A22F008}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5C4221AA-7C33-4AB7-B68B-3944576EEFD4}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HEAD" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="75">
   <si>
     <t>t_email_addr</t>
   </si>
@@ -261,6 +261,12 @@
   </si>
   <si>
     <t>-004900</t>
+  </si>
+  <si>
+    <t>t_noise_temp</t>
+  </si>
+  <si>
+    <t>T11</t>
   </si>
 </sst>
 </file>
@@ -270,7 +276,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -303,6 +309,12 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -356,7 +368,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -413,6 +425,22 @@
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -734,14 +762,14 @@
       <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -752,7 +780,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>59</v>
       </c>
@@ -761,7 +789,7 @@
       </c>
       <c r="C2" s="4">
         <f ca="1">TODAY()</f>
-        <v>45862</v>
+        <v>45863</v>
       </c>
     </row>
   </sheetData>
@@ -776,35 +804,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:U17"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:G2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.88671875" customWidth="1"/>
-    <col min="7" max="7" width="10.6640625" customWidth="1"/>
-    <col min="8" max="8" width="26.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" customWidth="1"/>
+    <col min="8" max="8" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.88671875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="51.44140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="51.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>4</v>
       </c>
@@ -869,7 +897,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>33</v>
       </c>
@@ -934,7 +962,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>33</v>
       </c>
@@ -999,7 +1027,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>33</v>
       </c>
@@ -1064,30 +1092,36 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A5" s="8"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="8"/>
-      <c r="L5" s="8"/>
-      <c r="M5" s="8"/>
-      <c r="N5" s="9"/>
-      <c r="O5" s="11"/>
-      <c r="P5" s="9"/>
-      <c r="Q5" s="9"/>
-      <c r="R5" s="8"/>
-      <c r="S5" s="8"/>
-      <c r="T5" s="8"/>
-      <c r="U5" s="8"/>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="13"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="24"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="21"/>
+      <c r="K5" s="20"/>
+      <c r="L5" s="20"/>
+      <c r="M5" s="20"/>
+      <c r="N5" s="21"/>
+      <c r="O5" s="24"/>
+      <c r="P5" s="21"/>
+      <c r="Q5" s="21"/>
+      <c r="R5" s="20"/>
+      <c r="S5" s="20"/>
+      <c r="T5" s="20"/>
+      <c r="U5" s="20"/>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="8"/>
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
@@ -1110,7 +1144,7 @@
       <c r="T6" s="8"/>
       <c r="U6" s="8"/>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
@@ -1133,7 +1167,7 @@
       <c r="T7" s="8"/>
       <c r="U7" s="8"/>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="8"/>
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
@@ -1156,7 +1190,7 @@
       <c r="T8" s="8"/>
       <c r="U8" s="8"/>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="8"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
@@ -1179,7 +1213,7 @@
       <c r="T9" s="8"/>
       <c r="U9" s="8"/>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="8"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
@@ -1202,7 +1236,7 @@
       <c r="T10" s="8"/>
       <c r="U10" s="8"/>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="8"/>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
@@ -1225,7 +1259,7 @@
       <c r="T11" s="8"/>
       <c r="U11" s="8"/>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="8"/>
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
@@ -1248,7 +1282,7 @@
       <c r="T12" s="8"/>
       <c r="U12" s="8"/>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="8"/>
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>
@@ -1271,7 +1305,7 @@
       <c r="T13" s="8"/>
       <c r="U13" s="8"/>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="8"/>
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
@@ -1294,7 +1328,7 @@
       <c r="T14" s="8"/>
       <c r="U14" s="8"/>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="8"/>
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>
@@ -1317,7 +1351,7 @@
       <c r="T15" s="8"/>
       <c r="U15" s="8"/>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="8"/>
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
@@ -1340,7 +1374,7 @@
       <c r="T16" s="8"/>
       <c r="U16" s="8"/>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" s="8"/>
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
@@ -1383,18 +1417,18 @@
       <selection activeCell="G3" sqref="F3:G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>7</v>
       </c>
@@ -1420,7 +1454,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>54</v>
       </c>
@@ -1447,7 +1481,7 @@
         <v>HF-GOV-0027</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>55</v>
       </c>
@@ -1474,7 +1508,7 @@
         <v>HF-GOV-0162</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>56</v>
       </c>
@@ -1510,22 +1544,24 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E6631C0-354E-4D0C-B7EC-713896124916}">
-  <dimension ref="A1:G822"/>
+  <dimension ref="A1:J822"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.44140625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="9.6640625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.88671875" style="18"/>
+    <col min="1" max="1" width="19.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" style="18"/>
+    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>7</v>
       </c>
@@ -1547,8 +1583,17 @@
       <c r="G1" s="17" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>54</v>
       </c>
@@ -1567,7 +1612,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>54</v>
       </c>
@@ -1586,7 +1631,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>54</v>
       </c>
@@ -1605,7 +1650,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>54</v>
       </c>
@@ -1624,7 +1669,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>55</v>
       </c>
@@ -1646,7 +1691,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>56</v>
       </c>
@@ -1663,2467 +1708,2467 @@
       <c r="E7" s="16"/>
       <c r="F7" s="16"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8"/>
       <c r="B8"/>
       <c r="C8"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9"/>
       <c r="B9"/>
       <c r="C9"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10"/>
       <c r="B10"/>
       <c r="C10"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11"/>
       <c r="B11"/>
       <c r="C11"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12"/>
       <c r="B12"/>
       <c r="C12"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13"/>
       <c r="B13"/>
       <c r="C13"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14"/>
       <c r="B14"/>
       <c r="C14"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15"/>
       <c r="B15"/>
       <c r="C15"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16"/>
       <c r="B16"/>
       <c r="C16"/>
     </row>
-    <row r="17" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G17" s="18"/>
     </row>
-    <row r="18" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G18" s="18"/>
     </row>
-    <row r="19" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G19" s="18"/>
     </row>
-    <row r="20" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G20" s="18"/>
     </row>
-    <row r="21" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G21" s="18"/>
     </row>
-    <row r="22" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G22" s="18"/>
     </row>
-    <row r="23" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G23" s="18"/>
     </row>
-    <row r="24" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G24" s="18"/>
     </row>
-    <row r="25" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G25" s="18"/>
     </row>
-    <row r="26" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G26" s="18"/>
     </row>
-    <row r="27" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G27" s="18"/>
     </row>
-    <row r="28" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G28" s="18"/>
     </row>
-    <row r="29" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G29" s="18"/>
     </row>
-    <row r="30" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G30" s="18"/>
     </row>
-    <row r="31" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G31" s="18"/>
     </row>
-    <row r="32" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G32" s="18"/>
     </row>
-    <row r="33" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G33" s="18"/>
     </row>
-    <row r="34" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G34" s="18"/>
     </row>
-    <row r="35" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G35" s="18"/>
     </row>
-    <row r="36" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G36" s="18"/>
     </row>
-    <row r="37" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G37" s="18"/>
     </row>
-    <row r="38" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G38" s="18"/>
     </row>
-    <row r="39" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G39" s="18"/>
     </row>
-    <row r="40" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G40" s="18"/>
     </row>
-    <row r="41" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G41" s="18"/>
     </row>
-    <row r="42" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G42" s="18"/>
     </row>
-    <row r="43" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G43" s="18"/>
     </row>
-    <row r="44" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G44" s="18"/>
     </row>
-    <row r="45" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G45" s="18"/>
     </row>
-    <row r="46" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G46" s="18"/>
     </row>
-    <row r="47" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G47" s="18"/>
     </row>
-    <row r="48" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G48" s="18"/>
     </row>
-    <row r="49" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G49" s="18"/>
     </row>
-    <row r="50" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G50" s="18"/>
     </row>
-    <row r="51" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G51" s="18"/>
     </row>
-    <row r="52" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G52" s="18"/>
     </row>
-    <row r="53" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G53" s="18"/>
     </row>
-    <row r="54" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G54" s="18"/>
     </row>
-    <row r="55" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G55" s="18"/>
     </row>
-    <row r="56" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G56" s="18"/>
     </row>
-    <row r="57" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G57" s="18"/>
     </row>
-    <row r="58" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G58" s="18"/>
     </row>
-    <row r="59" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G59" s="18"/>
     </row>
-    <row r="60" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G60" s="18"/>
     </row>
-    <row r="61" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G61" s="18"/>
     </row>
-    <row r="62" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G62" s="18"/>
     </row>
-    <row r="63" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G63" s="18"/>
     </row>
-    <row r="64" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G64" s="18"/>
     </row>
-    <row r="65" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G65" s="18"/>
     </row>
-    <row r="66" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G66" s="18"/>
     </row>
-    <row r="67" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G67" s="18"/>
     </row>
-    <row r="68" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G68" s="18"/>
     </row>
-    <row r="69" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G69" s="18"/>
     </row>
-    <row r="70" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G70" s="18"/>
     </row>
-    <row r="71" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G71" s="18"/>
     </row>
-    <row r="72" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G72" s="18"/>
     </row>
-    <row r="73" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G73" s="18"/>
     </row>
-    <row r="74" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G74" s="18"/>
     </row>
-    <row r="75" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G75" s="18"/>
     </row>
-    <row r="76" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G76" s="18"/>
     </row>
-    <row r="77" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G77" s="18"/>
     </row>
-    <row r="78" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G78" s="18"/>
     </row>
-    <row r="79" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G79" s="18"/>
     </row>
-    <row r="80" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G80" s="18"/>
     </row>
-    <row r="81" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G81" s="18"/>
     </row>
-    <row r="82" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G82" s="18"/>
     </row>
-    <row r="83" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G83" s="18"/>
     </row>
-    <row r="84" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G84" s="18"/>
     </row>
-    <row r="85" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G85" s="18"/>
     </row>
-    <row r="86" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G86" s="18"/>
     </row>
-    <row r="87" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G87" s="18"/>
     </row>
-    <row r="88" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G88" s="18"/>
     </row>
-    <row r="89" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G89" s="18"/>
     </row>
-    <row r="90" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G90" s="18"/>
     </row>
-    <row r="91" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G91" s="18"/>
     </row>
-    <row r="92" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G92" s="18"/>
     </row>
-    <row r="93" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G93" s="18"/>
     </row>
-    <row r="94" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G94" s="18"/>
     </row>
-    <row r="95" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G95" s="18"/>
     </row>
-    <row r="96" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G96" s="18"/>
     </row>
-    <row r="97" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G97" s="18"/>
     </row>
-    <row r="98" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G98" s="18"/>
     </row>
-    <row r="99" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G99" s="18"/>
     </row>
-    <row r="100" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G100" s="18"/>
     </row>
-    <row r="101" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G101" s="18"/>
     </row>
-    <row r="102" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G102" s="18"/>
     </row>
-    <row r="103" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G103" s="18"/>
     </row>
-    <row r="104" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G104" s="18"/>
     </row>
-    <row r="105" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G105" s="18"/>
     </row>
-    <row r="106" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G106" s="18"/>
     </row>
-    <row r="107" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G107" s="18"/>
     </row>
-    <row r="108" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G108" s="18"/>
     </row>
-    <row r="109" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G109" s="18"/>
     </row>
-    <row r="110" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G110" s="18"/>
     </row>
-    <row r="111" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G111" s="18"/>
     </row>
-    <row r="112" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G112" s="18"/>
     </row>
-    <row r="113" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G113" s="18"/>
     </row>
-    <row r="114" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G114" s="18"/>
     </row>
-    <row r="115" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G115" s="18"/>
     </row>
-    <row r="116" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G116" s="18"/>
     </row>
-    <row r="117" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G117" s="18"/>
     </row>
-    <row r="118" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G118" s="18"/>
     </row>
-    <row r="119" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G119" s="18"/>
     </row>
-    <row r="120" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G120" s="18"/>
     </row>
-    <row r="121" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G121" s="18"/>
     </row>
-    <row r="122" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G122" s="18"/>
     </row>
-    <row r="123" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G123" s="18"/>
     </row>
-    <row r="124" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G124" s="18"/>
     </row>
-    <row r="125" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G125" s="18"/>
     </row>
-    <row r="126" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G126" s="18"/>
     </row>
-    <row r="127" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G127" s="18"/>
     </row>
-    <row r="128" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G128" s="18"/>
     </row>
-    <row r="129" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G129" s="18"/>
     </row>
-    <row r="130" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G130" s="18"/>
     </row>
-    <row r="131" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G131" s="18"/>
     </row>
-    <row r="132" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G132" s="18"/>
     </row>
-    <row r="133" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G133" s="18"/>
     </row>
-    <row r="134" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G134" s="18"/>
     </row>
-    <row r="135" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G135" s="18"/>
     </row>
-    <row r="136" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G136" s="18"/>
     </row>
-    <row r="137" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G137" s="18"/>
     </row>
-    <row r="138" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G138" s="18"/>
     </row>
-    <row r="139" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G139" s="18"/>
     </row>
-    <row r="140" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G140" s="18"/>
     </row>
-    <row r="141" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G141" s="18"/>
     </row>
-    <row r="142" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G142" s="18"/>
     </row>
-    <row r="143" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G143" s="18"/>
     </row>
-    <row r="144" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G144" s="18"/>
     </row>
-    <row r="145" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G145" s="18"/>
     </row>
-    <row r="146" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G146" s="18"/>
     </row>
-    <row r="147" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G147" s="18"/>
     </row>
-    <row r="148" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G148" s="18"/>
     </row>
-    <row r="149" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G149" s="18"/>
     </row>
-    <row r="150" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G150" s="18"/>
     </row>
-    <row r="151" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G151" s="18"/>
     </row>
-    <row r="152" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G152" s="18"/>
     </row>
-    <row r="153" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G153" s="18"/>
     </row>
-    <row r="154" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G154" s="18"/>
     </row>
-    <row r="155" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G155" s="18"/>
     </row>
-    <row r="156" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G156" s="18"/>
     </row>
-    <row r="157" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G157" s="18"/>
     </row>
-    <row r="158" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G158" s="18"/>
     </row>
-    <row r="159" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="159" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G159" s="18"/>
     </row>
-    <row r="160" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="160" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G160" s="18"/>
     </row>
-    <row r="161" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="161" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G161" s="18"/>
     </row>
-    <row r="162" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="162" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G162" s="18"/>
     </row>
-    <row r="163" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="163" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G163" s="18"/>
     </row>
-    <row r="164" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G164" s="18"/>
     </row>
-    <row r="165" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G165" s="18"/>
     </row>
-    <row r="166" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G166" s="18"/>
     </row>
-    <row r="167" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G167" s="18"/>
     </row>
-    <row r="168" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G168" s="18"/>
     </row>
-    <row r="169" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="169" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G169" s="18"/>
     </row>
-    <row r="170" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="170" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G170" s="18"/>
     </row>
-    <row r="171" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="171" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G171" s="18"/>
     </row>
-    <row r="172" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="172" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G172" s="18"/>
     </row>
-    <row r="173" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="173" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G173" s="18"/>
     </row>
-    <row r="174" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="174" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G174" s="18"/>
     </row>
-    <row r="175" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="175" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G175" s="18"/>
     </row>
-    <row r="176" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="176" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G176" s="18"/>
     </row>
-    <row r="177" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="177" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G177" s="18"/>
     </row>
-    <row r="178" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="178" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G178" s="18"/>
     </row>
-    <row r="179" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="179" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G179" s="18"/>
     </row>
-    <row r="180" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="180" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G180" s="18"/>
     </row>
-    <row r="181" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="181" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G181" s="18"/>
     </row>
-    <row r="182" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="182" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G182" s="18"/>
     </row>
-    <row r="183" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="183" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G183" s="18"/>
     </row>
-    <row r="184" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="184" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G184" s="18"/>
     </row>
-    <row r="185" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="185" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G185" s="18"/>
     </row>
-    <row r="186" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="186" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G186" s="18"/>
     </row>
-    <row r="187" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="187" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G187" s="18"/>
     </row>
-    <row r="188" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="188" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G188" s="18"/>
     </row>
-    <row r="189" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="189" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G189" s="18"/>
     </row>
-    <row r="190" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="190" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G190" s="18"/>
     </row>
-    <row r="191" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="191" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G191" s="18"/>
     </row>
-    <row r="192" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="192" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G192" s="18"/>
     </row>
-    <row r="193" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="193" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G193" s="18"/>
     </row>
-    <row r="194" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="194" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G194" s="18"/>
     </row>
-    <row r="195" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="195" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G195" s="18"/>
     </row>
-    <row r="196" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="196" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G196" s="18"/>
     </row>
-    <row r="197" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="197" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G197" s="18"/>
     </row>
-    <row r="198" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="198" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G198" s="18"/>
     </row>
-    <row r="199" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="199" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G199" s="18"/>
     </row>
-    <row r="200" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="200" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G200" s="18"/>
     </row>
-    <row r="201" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="201" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G201" s="18"/>
     </row>
-    <row r="202" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="202" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G202" s="18"/>
     </row>
-    <row r="203" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="203" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G203" s="18"/>
     </row>
-    <row r="204" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="204" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G204" s="18"/>
     </row>
-    <row r="205" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="205" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G205" s="18"/>
     </row>
-    <row r="206" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="206" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G206" s="18"/>
     </row>
-    <row r="207" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="207" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G207" s="18"/>
     </row>
-    <row r="208" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="208" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G208" s="18"/>
     </row>
-    <row r="209" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="209" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G209" s="18"/>
     </row>
-    <row r="210" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="210" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G210" s="18"/>
     </row>
-    <row r="211" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="211" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G211" s="18"/>
     </row>
-    <row r="212" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="212" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G212" s="18"/>
     </row>
-    <row r="213" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="213" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G213" s="18"/>
     </row>
-    <row r="214" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="214" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G214" s="18"/>
     </row>
-    <row r="215" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="215" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G215" s="18"/>
     </row>
-    <row r="216" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="216" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G216" s="18"/>
     </row>
-    <row r="217" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="217" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G217" s="18"/>
     </row>
-    <row r="218" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="218" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G218" s="18"/>
     </row>
-    <row r="219" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="219" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G219" s="18"/>
     </row>
-    <row r="220" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="220" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G220" s="18"/>
     </row>
-    <row r="221" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="221" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G221" s="18"/>
     </row>
-    <row r="222" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="222" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G222" s="18"/>
     </row>
-    <row r="223" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="223" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G223" s="18"/>
     </row>
-    <row r="224" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="224" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G224" s="18"/>
     </row>
-    <row r="225" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="225" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G225" s="18"/>
     </row>
-    <row r="226" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="226" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G226" s="18"/>
     </row>
-    <row r="227" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="227" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G227" s="18"/>
     </row>
-    <row r="228" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="228" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G228" s="18"/>
     </row>
-    <row r="229" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="229" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G229" s="18"/>
     </row>
-    <row r="230" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="230" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G230" s="18"/>
     </row>
-    <row r="231" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="231" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G231" s="18"/>
     </row>
-    <row r="232" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="232" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G232" s="18"/>
     </row>
-    <row r="233" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="233" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G233" s="18"/>
     </row>
-    <row r="234" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="234" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G234" s="18"/>
     </row>
-    <row r="235" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="235" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G235" s="18"/>
     </row>
-    <row r="236" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="236" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G236" s="18"/>
     </row>
-    <row r="237" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="237" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G237" s="18"/>
     </row>
-    <row r="238" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="238" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G238" s="18"/>
     </row>
-    <row r="239" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="239" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G239" s="18"/>
     </row>
-    <row r="240" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="240" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G240" s="18"/>
     </row>
-    <row r="241" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="241" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G241" s="18"/>
     </row>
-    <row r="242" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="242" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G242" s="18"/>
     </row>
-    <row r="243" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="243" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G243" s="18"/>
     </row>
-    <row r="244" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="244" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G244" s="18"/>
     </row>
-    <row r="245" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="245" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G245" s="18"/>
     </row>
-    <row r="246" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="246" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G246" s="18"/>
     </row>
-    <row r="247" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="247" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G247" s="18"/>
     </row>
-    <row r="248" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="248" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G248" s="18"/>
     </row>
-    <row r="249" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="249" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G249" s="18"/>
     </row>
-    <row r="250" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="250" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G250" s="18"/>
     </row>
-    <row r="251" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="251" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G251" s="18"/>
     </row>
-    <row r="252" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="252" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G252" s="18"/>
     </row>
-    <row r="253" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="253" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G253" s="18"/>
     </row>
-    <row r="254" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="254" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G254" s="18"/>
     </row>
-    <row r="255" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="255" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G255" s="18"/>
     </row>
-    <row r="256" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="256" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G256" s="18"/>
     </row>
-    <row r="257" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="257" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G257" s="18"/>
     </row>
-    <row r="258" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="258" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G258" s="18"/>
     </row>
-    <row r="259" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="259" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G259" s="18"/>
     </row>
-    <row r="260" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="260" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G260" s="18"/>
     </row>
-    <row r="261" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="261" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G261" s="18"/>
     </row>
-    <row r="262" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="262" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G262" s="18"/>
     </row>
-    <row r="263" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="263" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G263" s="18"/>
     </row>
-    <row r="264" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="264" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G264" s="18"/>
     </row>
-    <row r="265" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="265" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G265" s="18"/>
     </row>
-    <row r="266" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="266" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G266" s="18"/>
     </row>
-    <row r="267" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="267" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G267" s="18"/>
     </row>
-    <row r="268" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="268" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G268" s="18"/>
     </row>
-    <row r="269" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="269" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G269" s="18"/>
     </row>
-    <row r="270" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="270" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G270" s="18"/>
     </row>
-    <row r="271" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="271" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G271" s="18"/>
     </row>
-    <row r="272" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="272" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G272" s="18"/>
     </row>
-    <row r="273" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="273" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G273" s="18"/>
     </row>
-    <row r="274" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="274" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G274" s="18"/>
     </row>
-    <row r="275" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="275" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G275" s="18"/>
     </row>
-    <row r="276" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="276" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G276" s="18"/>
     </row>
-    <row r="277" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="277" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G277" s="18"/>
     </row>
-    <row r="278" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="278" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G278" s="18"/>
     </row>
-    <row r="279" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="279" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G279" s="18"/>
     </row>
-    <row r="280" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="280" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G280" s="18"/>
     </row>
-    <row r="281" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="281" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G281" s="18"/>
     </row>
-    <row r="282" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="282" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G282" s="18"/>
     </row>
-    <row r="283" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="283" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G283" s="18"/>
     </row>
-    <row r="284" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="284" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G284" s="18"/>
     </row>
-    <row r="285" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="285" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G285" s="18"/>
     </row>
-    <row r="286" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="286" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G286" s="18"/>
     </row>
-    <row r="287" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="287" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G287" s="18"/>
     </row>
-    <row r="288" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="288" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G288" s="18"/>
     </row>
-    <row r="289" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="289" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G289" s="18"/>
     </row>
-    <row r="290" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="290" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G290" s="18"/>
     </row>
-    <row r="291" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="291" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G291" s="18"/>
     </row>
-    <row r="292" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="292" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G292" s="18"/>
     </row>
-    <row r="293" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="293" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G293" s="18"/>
     </row>
-    <row r="294" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="294" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G294" s="18"/>
     </row>
-    <row r="295" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="295" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G295" s="18"/>
     </row>
-    <row r="296" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="296" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G296" s="18"/>
     </row>
-    <row r="297" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="297" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G297" s="18"/>
     </row>
-    <row r="298" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="298" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G298" s="18"/>
     </row>
-    <row r="299" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="299" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G299" s="18"/>
     </row>
-    <row r="300" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="300" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G300" s="18"/>
     </row>
-    <row r="301" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="301" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G301" s="18"/>
     </row>
-    <row r="302" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="302" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G302" s="18"/>
     </row>
-    <row r="303" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="303" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G303" s="18"/>
     </row>
-    <row r="304" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="304" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G304" s="18"/>
     </row>
-    <row r="305" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="305" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G305" s="18"/>
     </row>
-    <row r="306" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="306" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G306" s="18"/>
     </row>
-    <row r="307" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="307" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G307" s="18"/>
     </row>
-    <row r="308" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="308" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G308" s="18"/>
     </row>
-    <row r="309" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="309" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G309" s="18"/>
     </row>
-    <row r="310" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="310" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G310" s="18"/>
     </row>
-    <row r="311" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="311" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G311" s="18"/>
     </row>
-    <row r="312" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="312" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G312" s="18"/>
     </row>
-    <row r="313" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="313" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G313" s="18"/>
     </row>
-    <row r="314" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="314" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G314" s="18"/>
     </row>
-    <row r="315" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="315" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G315" s="18"/>
     </row>
-    <row r="316" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="316" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G316" s="18"/>
     </row>
-    <row r="317" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="317" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G317" s="18"/>
     </row>
-    <row r="318" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="318" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G318" s="18"/>
     </row>
-    <row r="319" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="319" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G319" s="18"/>
     </row>
-    <row r="320" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="320" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G320" s="18"/>
     </row>
-    <row r="321" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="321" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G321" s="18"/>
     </row>
-    <row r="322" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="322" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G322" s="18"/>
     </row>
-    <row r="323" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="323" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G323" s="18"/>
     </row>
-    <row r="324" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="324" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G324" s="18"/>
     </row>
-    <row r="325" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="325" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G325" s="18"/>
     </row>
-    <row r="326" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="326" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G326" s="18"/>
     </row>
-    <row r="327" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="327" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G327" s="18"/>
     </row>
-    <row r="328" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="328" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G328" s="18"/>
     </row>
-    <row r="329" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="329" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G329" s="18"/>
     </row>
-    <row r="330" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="330" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G330" s="18"/>
     </row>
-    <row r="331" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="331" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G331" s="18"/>
     </row>
-    <row r="332" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="332" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G332" s="18"/>
     </row>
-    <row r="333" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="333" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G333" s="18"/>
     </row>
-    <row r="334" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="334" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G334" s="18"/>
     </row>
-    <row r="335" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="335" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G335" s="18"/>
     </row>
-    <row r="336" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="336" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G336" s="18"/>
     </row>
-    <row r="337" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="337" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G337" s="18"/>
     </row>
-    <row r="338" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="338" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G338" s="18"/>
     </row>
-    <row r="339" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="339" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G339" s="18"/>
     </row>
-    <row r="340" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="340" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G340" s="18"/>
     </row>
-    <row r="341" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="341" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G341" s="18"/>
     </row>
-    <row r="342" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="342" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G342" s="18"/>
     </row>
-    <row r="343" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="343" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G343" s="18"/>
     </row>
-    <row r="344" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="344" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G344" s="18"/>
     </row>
-    <row r="345" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="345" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G345" s="18"/>
     </row>
-    <row r="346" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="346" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G346" s="18"/>
     </row>
-    <row r="347" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="347" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G347" s="18"/>
     </row>
-    <row r="348" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="348" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G348" s="18"/>
     </row>
-    <row r="349" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="349" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G349" s="18"/>
     </row>
-    <row r="350" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="350" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G350" s="18"/>
     </row>
-    <row r="351" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="351" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G351" s="18"/>
     </row>
-    <row r="352" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="352" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G352" s="18"/>
     </row>
-    <row r="353" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="353" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G353" s="18"/>
     </row>
-    <row r="354" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="354" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G354" s="18"/>
     </row>
-    <row r="355" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="355" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G355" s="18"/>
     </row>
-    <row r="356" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="356" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G356" s="18"/>
     </row>
-    <row r="357" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="357" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G357" s="18"/>
     </row>
-    <row r="358" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="358" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G358" s="18"/>
     </row>
-    <row r="359" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="359" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G359" s="18"/>
     </row>
-    <row r="360" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="360" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G360" s="18"/>
     </row>
-    <row r="361" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="361" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G361" s="18"/>
     </row>
-    <row r="362" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="362" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G362" s="18"/>
     </row>
-    <row r="363" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="363" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G363" s="18"/>
     </row>
-    <row r="364" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="364" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G364" s="18"/>
     </row>
-    <row r="365" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="365" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G365" s="18"/>
     </row>
-    <row r="366" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="366" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G366" s="18"/>
     </row>
-    <row r="367" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="367" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G367" s="18"/>
     </row>
-    <row r="368" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="368" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G368" s="18"/>
     </row>
-    <row r="369" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="369" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G369" s="18"/>
     </row>
-    <row r="370" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="370" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G370" s="18"/>
     </row>
-    <row r="371" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="371" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G371" s="18"/>
     </row>
-    <row r="372" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="372" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G372" s="18"/>
     </row>
-    <row r="373" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="373" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G373" s="18"/>
     </row>
-    <row r="374" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="374" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G374" s="18"/>
     </row>
-    <row r="375" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="375" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G375" s="18"/>
     </row>
-    <row r="376" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="376" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G376" s="18"/>
     </row>
-    <row r="377" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="377" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G377" s="18"/>
     </row>
-    <row r="378" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="378" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G378" s="18"/>
     </row>
-    <row r="379" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="379" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G379" s="18"/>
     </row>
-    <row r="380" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="380" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G380" s="18"/>
     </row>
-    <row r="381" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="381" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G381" s="18"/>
     </row>
-    <row r="382" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="382" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G382" s="18"/>
     </row>
-    <row r="383" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="383" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G383" s="18"/>
     </row>
-    <row r="384" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="384" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G384" s="18"/>
     </row>
-    <row r="385" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="385" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G385" s="18"/>
     </row>
-    <row r="386" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="386" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G386" s="18"/>
     </row>
-    <row r="387" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="387" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G387" s="18"/>
     </row>
-    <row r="388" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="388" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G388" s="18"/>
     </row>
-    <row r="389" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="389" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G389" s="18"/>
     </row>
-    <row r="390" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="390" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G390" s="18"/>
     </row>
-    <row r="391" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="391" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G391" s="18"/>
     </row>
-    <row r="392" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="392" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G392" s="18"/>
     </row>
-    <row r="393" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="393" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G393" s="18"/>
     </row>
-    <row r="394" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="394" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G394" s="18"/>
     </row>
-    <row r="395" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="395" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G395" s="18"/>
     </row>
-    <row r="396" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="396" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G396" s="18"/>
     </row>
-    <row r="397" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="397" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G397" s="18"/>
     </row>
-    <row r="398" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="398" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G398" s="18"/>
     </row>
-    <row r="399" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="399" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G399" s="18"/>
     </row>
-    <row r="400" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="400" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G400" s="18"/>
     </row>
-    <row r="401" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="401" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G401" s="18"/>
     </row>
-    <row r="402" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="402" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G402" s="18"/>
     </row>
-    <row r="403" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="403" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G403" s="18"/>
     </row>
-    <row r="404" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="404" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G404" s="18"/>
     </row>
-    <row r="405" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="405" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G405" s="18"/>
     </row>
-    <row r="406" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="406" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G406" s="18"/>
     </row>
-    <row r="407" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="407" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G407" s="18"/>
     </row>
-    <row r="408" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="408" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G408" s="18"/>
     </row>
-    <row r="409" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="409" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G409" s="18"/>
     </row>
-    <row r="410" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="410" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G410" s="18"/>
     </row>
-    <row r="411" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="411" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G411" s="18"/>
     </row>
-    <row r="412" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="412" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G412" s="18"/>
     </row>
-    <row r="413" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="413" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G413" s="18"/>
     </row>
-    <row r="414" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="414" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G414" s="18"/>
     </row>
-    <row r="415" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="415" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G415" s="18"/>
     </row>
-    <row r="416" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="416" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G416" s="18"/>
     </row>
-    <row r="417" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="417" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G417" s="18"/>
     </row>
-    <row r="418" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="418" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G418" s="18"/>
     </row>
-    <row r="419" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="419" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G419" s="18"/>
     </row>
-    <row r="420" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="420" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G420" s="18"/>
     </row>
-    <row r="421" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="421" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G421" s="18"/>
     </row>
-    <row r="422" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="422" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G422" s="18"/>
     </row>
-    <row r="423" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="423" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G423" s="18"/>
     </row>
-    <row r="424" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="424" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G424" s="18"/>
     </row>
-    <row r="425" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="425" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G425" s="18"/>
     </row>
-    <row r="426" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="426" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G426" s="18"/>
     </row>
-    <row r="427" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="427" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G427" s="18"/>
     </row>
-    <row r="428" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="428" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G428" s="18"/>
     </row>
-    <row r="429" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="429" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G429" s="18"/>
     </row>
-    <row r="430" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="430" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G430" s="18"/>
     </row>
-    <row r="431" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="431" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G431" s="18"/>
     </row>
-    <row r="432" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="432" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G432" s="18"/>
     </row>
-    <row r="433" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="433" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G433" s="18"/>
     </row>
-    <row r="434" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="434" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G434" s="18"/>
     </row>
-    <row r="435" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="435" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G435" s="18"/>
     </row>
-    <row r="436" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="436" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G436" s="18"/>
     </row>
-    <row r="437" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="437" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G437" s="18"/>
     </row>
-    <row r="438" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="438" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G438" s="18"/>
     </row>
-    <row r="439" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="439" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G439" s="18"/>
     </row>
-    <row r="440" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="440" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G440" s="18"/>
     </row>
-    <row r="441" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="441" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G441" s="18"/>
     </row>
-    <row r="442" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="442" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G442" s="18"/>
     </row>
-    <row r="443" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="443" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G443" s="18"/>
     </row>
-    <row r="444" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="444" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G444" s="18"/>
     </row>
-    <row r="445" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="445" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G445" s="18"/>
     </row>
-    <row r="446" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="446" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G446" s="18"/>
     </row>
-    <row r="447" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="447" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G447" s="18"/>
     </row>
-    <row r="448" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="448" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G448" s="18"/>
     </row>
-    <row r="449" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="449" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G449" s="18"/>
     </row>
-    <row r="450" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="450" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G450" s="18"/>
     </row>
-    <row r="451" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="451" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G451" s="18"/>
     </row>
-    <row r="452" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="452" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G452" s="18"/>
     </row>
-    <row r="453" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="453" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G453" s="18"/>
     </row>
-    <row r="454" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="454" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G454" s="18"/>
     </row>
-    <row r="455" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="455" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G455" s="18"/>
     </row>
-    <row r="456" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="456" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G456" s="18"/>
     </row>
-    <row r="457" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="457" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G457" s="18"/>
     </row>
-    <row r="458" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="458" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G458" s="18"/>
     </row>
-    <row r="459" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="459" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G459" s="18"/>
     </row>
-    <row r="460" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="460" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G460" s="18"/>
     </row>
-    <row r="461" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="461" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G461" s="18"/>
     </row>
-    <row r="462" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="462" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G462" s="18"/>
     </row>
-    <row r="463" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="463" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G463" s="18"/>
     </row>
-    <row r="464" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="464" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G464" s="18"/>
     </row>
-    <row r="465" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="465" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G465" s="18"/>
     </row>
-    <row r="466" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="466" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G466" s="18"/>
     </row>
-    <row r="467" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="467" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G467" s="18"/>
     </row>
-    <row r="468" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="468" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G468" s="18"/>
     </row>
-    <row r="469" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="469" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G469" s="18"/>
     </row>
-    <row r="470" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="470" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G470" s="18"/>
     </row>
-    <row r="471" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="471" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G471" s="18"/>
     </row>
-    <row r="472" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="472" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G472" s="18"/>
     </row>
-    <row r="473" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="473" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G473" s="18"/>
     </row>
-    <row r="474" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="474" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G474" s="18"/>
     </row>
-    <row r="475" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="475" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G475" s="18"/>
     </row>
-    <row r="476" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="476" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G476" s="18"/>
     </row>
-    <row r="477" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="477" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G477" s="18"/>
     </row>
-    <row r="478" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="478" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G478" s="18"/>
     </row>
-    <row r="479" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="479" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G479" s="18"/>
     </row>
-    <row r="480" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="480" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G480" s="18"/>
     </row>
-    <row r="481" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="481" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G481" s="18"/>
     </row>
-    <row r="482" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="482" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G482" s="18"/>
     </row>
-    <row r="483" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="483" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G483" s="18"/>
     </row>
-    <row r="484" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="484" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G484" s="18"/>
     </row>
-    <row r="485" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="485" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G485" s="18"/>
     </row>
-    <row r="486" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="486" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G486" s="18"/>
     </row>
-    <row r="487" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="487" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G487" s="18"/>
     </row>
-    <row r="488" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="488" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G488" s="18"/>
     </row>
-    <row r="489" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="489" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G489" s="18"/>
     </row>
-    <row r="490" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="490" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G490" s="18"/>
     </row>
-    <row r="491" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="491" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G491" s="18"/>
     </row>
-    <row r="492" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="492" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G492" s="18"/>
     </row>
-    <row r="493" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="493" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G493" s="18"/>
     </row>
-    <row r="494" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="494" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G494" s="18"/>
     </row>
-    <row r="495" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="495" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G495" s="18"/>
     </row>
-    <row r="496" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="496" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G496" s="18"/>
     </row>
-    <row r="497" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="497" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G497" s="18"/>
     </row>
-    <row r="498" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="498" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G498" s="18"/>
     </row>
-    <row r="499" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="499" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G499" s="18"/>
     </row>
-    <row r="500" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="500" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G500" s="18"/>
     </row>
-    <row r="501" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="501" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G501" s="18"/>
     </row>
-    <row r="502" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="502" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G502" s="18"/>
     </row>
-    <row r="503" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="503" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G503" s="18"/>
     </row>
-    <row r="504" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="504" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G504" s="18"/>
     </row>
-    <row r="505" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="505" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G505" s="18"/>
     </row>
-    <row r="506" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="506" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G506" s="18"/>
     </row>
-    <row r="507" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="507" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G507" s="18"/>
     </row>
-    <row r="508" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="508" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G508" s="18"/>
     </row>
-    <row r="509" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="509" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G509" s="18"/>
     </row>
-    <row r="510" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="510" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G510" s="18"/>
     </row>
-    <row r="511" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="511" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G511" s="18"/>
     </row>
-    <row r="512" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="512" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G512" s="18"/>
     </row>
-    <row r="513" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="513" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G513" s="18"/>
     </row>
-    <row r="514" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="514" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G514" s="18"/>
     </row>
-    <row r="515" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="515" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G515" s="18"/>
     </row>
-    <row r="516" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="516" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G516" s="18"/>
     </row>
-    <row r="517" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="517" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G517" s="18"/>
     </row>
-    <row r="518" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="518" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G518" s="18"/>
     </row>
-    <row r="519" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="519" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G519" s="18"/>
     </row>
-    <row r="520" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="520" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G520" s="18"/>
     </row>
-    <row r="521" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="521" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G521" s="18"/>
     </row>
-    <row r="522" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="522" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G522" s="18"/>
     </row>
-    <row r="523" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="523" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G523" s="18"/>
     </row>
-    <row r="524" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="524" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G524" s="18"/>
     </row>
-    <row r="525" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="525" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G525" s="18"/>
     </row>
-    <row r="526" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="526" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G526" s="18"/>
     </row>
-    <row r="527" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="527" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G527" s="18"/>
     </row>
-    <row r="528" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="528" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G528" s="18"/>
     </row>
-    <row r="529" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="529" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G529" s="18"/>
     </row>
-    <row r="530" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="530" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G530" s="18"/>
     </row>
-    <row r="531" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="531" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G531" s="18"/>
     </row>
-    <row r="532" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="532" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G532" s="18"/>
     </row>
-    <row r="533" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="533" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G533" s="18"/>
     </row>
-    <row r="534" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="534" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G534" s="18"/>
     </row>
-    <row r="535" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="535" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G535" s="18"/>
     </row>
-    <row r="536" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="536" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G536" s="18"/>
     </row>
-    <row r="537" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="537" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G537" s="18"/>
     </row>
-    <row r="538" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="538" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G538" s="18"/>
     </row>
-    <row r="539" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="539" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G539" s="18"/>
     </row>
-    <row r="540" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="540" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G540" s="18"/>
     </row>
-    <row r="541" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="541" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G541" s="18"/>
     </row>
-    <row r="542" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="542" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G542" s="18"/>
     </row>
-    <row r="543" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="543" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G543" s="18"/>
     </row>
-    <row r="544" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="544" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G544" s="18"/>
     </row>
-    <row r="545" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="545" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G545" s="18"/>
     </row>
-    <row r="546" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="546" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G546" s="18"/>
     </row>
-    <row r="547" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="547" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G547" s="18"/>
     </row>
-    <row r="548" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="548" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G548" s="18"/>
     </row>
-    <row r="549" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="549" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G549" s="18"/>
     </row>
-    <row r="550" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="550" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G550" s="18"/>
     </row>
-    <row r="551" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="551" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G551" s="18"/>
     </row>
-    <row r="552" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="552" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G552" s="18"/>
     </row>
-    <row r="553" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="553" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G553" s="18"/>
     </row>
-    <row r="554" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="554" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G554" s="18"/>
     </row>
-    <row r="555" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="555" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G555" s="18"/>
     </row>
-    <row r="556" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="556" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G556" s="18"/>
     </row>
-    <row r="557" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="557" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G557" s="18"/>
     </row>
-    <row r="558" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="558" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G558" s="18"/>
     </row>
-    <row r="559" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="559" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G559" s="18"/>
     </row>
-    <row r="560" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="560" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G560" s="18"/>
     </row>
-    <row r="561" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="561" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G561" s="18"/>
     </row>
-    <row r="562" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="562" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G562" s="18"/>
     </row>
-    <row r="563" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="563" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G563" s="18"/>
     </row>
-    <row r="564" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="564" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G564" s="18"/>
     </row>
-    <row r="565" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="565" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G565" s="18"/>
     </row>
-    <row r="566" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="566" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G566" s="18"/>
     </row>
-    <row r="567" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="567" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G567" s="18"/>
     </row>
-    <row r="568" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="568" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G568" s="18"/>
     </row>
-    <row r="569" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="569" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G569" s="18"/>
     </row>
-    <row r="570" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="570" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G570" s="18"/>
     </row>
-    <row r="571" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="571" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G571" s="18"/>
     </row>
-    <row r="572" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="572" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G572" s="18"/>
     </row>
-    <row r="573" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="573" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G573" s="18"/>
     </row>
-    <row r="574" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="574" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G574" s="18"/>
     </row>
-    <row r="575" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="575" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G575" s="18"/>
     </row>
-    <row r="576" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="576" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G576" s="18"/>
     </row>
-    <row r="577" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="577" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G577" s="18"/>
     </row>
-    <row r="578" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="578" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G578" s="18"/>
     </row>
-    <row r="579" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="579" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G579" s="18"/>
     </row>
-    <row r="580" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="580" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G580" s="18"/>
     </row>
-    <row r="581" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="581" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G581" s="18"/>
     </row>
-    <row r="582" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="582" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G582" s="18"/>
     </row>
-    <row r="583" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="583" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G583" s="18"/>
     </row>
-    <row r="584" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="584" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G584" s="18"/>
     </row>
-    <row r="585" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="585" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G585" s="18"/>
     </row>
-    <row r="586" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="586" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G586" s="18"/>
     </row>
-    <row r="587" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="587" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G587" s="18"/>
     </row>
-    <row r="588" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="588" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G588" s="18"/>
     </row>
-    <row r="589" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="589" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G589" s="18"/>
     </row>
-    <row r="590" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="590" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G590" s="18"/>
     </row>
-    <row r="591" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="591" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G591" s="18"/>
     </row>
-    <row r="592" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="592" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G592" s="18"/>
     </row>
-    <row r="593" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="593" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G593" s="18"/>
     </row>
-    <row r="594" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="594" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G594" s="18"/>
     </row>
-    <row r="595" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="595" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G595" s="18"/>
     </row>
-    <row r="596" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="596" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G596" s="18"/>
     </row>
-    <row r="597" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="597" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G597" s="18"/>
     </row>
-    <row r="598" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="598" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G598" s="18"/>
     </row>
-    <row r="599" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="599" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G599" s="18"/>
     </row>
-    <row r="600" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="600" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G600" s="18"/>
     </row>
-    <row r="601" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="601" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G601" s="18"/>
     </row>
-    <row r="602" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="602" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G602" s="18"/>
     </row>
-    <row r="603" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="603" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G603" s="18"/>
     </row>
-    <row r="604" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="604" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G604" s="18"/>
     </row>
-    <row r="605" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="605" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G605" s="18"/>
     </row>
-    <row r="606" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="606" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G606" s="18"/>
     </row>
-    <row r="607" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="607" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G607" s="18"/>
     </row>
-    <row r="608" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="608" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G608" s="18"/>
     </row>
-    <row r="609" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="609" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G609" s="18"/>
     </row>
-    <row r="610" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="610" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G610" s="18"/>
     </row>
-    <row r="611" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="611" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G611" s="18"/>
     </row>
-    <row r="612" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="612" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G612" s="18"/>
     </row>
-    <row r="613" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="613" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G613" s="18"/>
     </row>
-    <row r="614" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="614" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G614" s="18"/>
     </row>
-    <row r="615" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="615" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G615" s="18"/>
     </row>
-    <row r="616" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="616" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G616" s="18"/>
     </row>
-    <row r="617" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="617" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G617" s="18"/>
     </row>
-    <row r="618" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="618" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G618" s="18"/>
     </row>
-    <row r="619" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="619" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G619" s="18"/>
     </row>
-    <row r="620" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="620" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G620" s="18"/>
     </row>
-    <row r="621" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="621" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G621" s="18"/>
     </row>
-    <row r="622" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="622" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G622" s="18"/>
     </row>
-    <row r="623" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="623" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G623" s="18"/>
     </row>
-    <row r="624" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="624" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G624" s="18"/>
     </row>
-    <row r="625" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="625" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G625" s="18"/>
     </row>
-    <row r="626" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="626" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G626" s="18"/>
     </row>
-    <row r="627" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="627" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G627" s="18"/>
     </row>
-    <row r="628" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="628" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G628" s="18"/>
     </row>
-    <row r="629" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="629" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G629" s="18"/>
     </row>
-    <row r="630" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="630" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G630" s="18"/>
     </row>
-    <row r="631" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="631" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G631" s="18"/>
     </row>
-    <row r="632" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="632" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G632" s="18"/>
     </row>
-    <row r="633" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="633" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G633" s="18"/>
     </row>
-    <row r="634" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="634" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G634" s="18"/>
     </row>
-    <row r="635" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="635" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G635" s="18"/>
     </row>
-    <row r="636" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="636" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G636" s="18"/>
     </row>
-    <row r="637" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="637" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G637" s="18"/>
     </row>
-    <row r="638" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="638" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G638" s="18"/>
     </row>
-    <row r="639" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="639" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G639" s="18"/>
     </row>
-    <row r="640" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="640" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G640" s="18"/>
     </row>
-    <row r="641" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="641" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G641" s="18"/>
     </row>
-    <row r="642" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="642" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G642" s="18"/>
     </row>
-    <row r="643" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="643" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G643" s="18"/>
     </row>
-    <row r="644" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="644" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G644" s="18"/>
     </row>
-    <row r="645" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="645" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G645" s="18"/>
     </row>
-    <row r="646" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="646" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G646" s="18"/>
     </row>
-    <row r="647" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="647" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G647" s="18"/>
     </row>
-    <row r="648" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="648" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G648" s="18"/>
     </row>
-    <row r="649" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="649" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G649" s="18"/>
     </row>
-    <row r="650" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="650" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G650" s="18"/>
     </row>
-    <row r="651" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="651" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G651" s="18"/>
     </row>
-    <row r="652" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="652" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G652" s="18"/>
     </row>
-    <row r="653" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="653" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G653" s="18"/>
     </row>
-    <row r="654" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="654" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G654" s="18"/>
     </row>
-    <row r="655" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="655" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G655" s="18"/>
     </row>
-    <row r="656" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="656" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G656" s="18"/>
     </row>
-    <row r="657" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="657" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G657" s="18"/>
     </row>
-    <row r="658" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="658" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G658" s="18"/>
     </row>
-    <row r="659" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="659" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G659" s="18"/>
     </row>
-    <row r="660" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="660" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G660" s="18"/>
     </row>
-    <row r="661" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="661" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G661" s="18"/>
     </row>
-    <row r="662" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="662" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G662" s="18"/>
     </row>
-    <row r="663" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="663" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G663" s="18"/>
     </row>
-    <row r="664" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="664" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G664" s="18"/>
     </row>
-    <row r="665" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="665" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G665" s="18"/>
     </row>
-    <row r="666" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="666" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G666" s="18"/>
     </row>
-    <row r="667" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="667" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G667" s="18"/>
     </row>
-    <row r="668" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="668" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G668" s="18"/>
     </row>
-    <row r="669" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="669" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G669" s="18"/>
     </row>
-    <row r="670" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="670" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G670" s="18"/>
     </row>
-    <row r="671" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="671" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G671" s="18"/>
     </row>
-    <row r="672" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="672" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G672" s="18"/>
     </row>
-    <row r="673" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="673" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G673" s="18"/>
     </row>
-    <row r="674" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="674" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G674" s="18"/>
     </row>
-    <row r="675" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="675" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G675" s="18"/>
     </row>
-    <row r="676" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="676" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G676" s="18"/>
     </row>
-    <row r="677" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="677" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G677" s="18"/>
     </row>
-    <row r="678" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="678" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G678" s="18"/>
     </row>
-    <row r="679" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="679" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G679" s="18"/>
     </row>
-    <row r="680" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="680" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G680" s="18"/>
     </row>
-    <row r="681" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="681" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G681" s="18"/>
     </row>
-    <row r="682" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="682" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G682" s="18"/>
     </row>
-    <row r="683" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="683" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G683" s="18"/>
     </row>
-    <row r="684" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="684" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G684" s="18"/>
     </row>
-    <row r="685" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="685" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G685" s="18"/>
     </row>
-    <row r="686" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="686" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G686" s="18"/>
     </row>
-    <row r="687" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="687" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G687" s="18"/>
     </row>
-    <row r="688" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="688" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G688" s="18"/>
     </row>
-    <row r="689" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="689" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G689" s="18"/>
     </row>
-    <row r="690" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="690" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G690" s="18"/>
     </row>
-    <row r="691" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="691" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G691" s="18"/>
     </row>
-    <row r="692" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="692" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G692" s="18"/>
     </row>
-    <row r="693" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="693" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G693" s="18"/>
     </row>
-    <row r="694" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="694" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G694" s="18"/>
     </row>
-    <row r="695" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="695" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G695" s="18"/>
     </row>
-    <row r="696" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="696" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G696" s="18"/>
     </row>
-    <row r="697" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="697" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G697" s="18"/>
     </row>
-    <row r="698" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="698" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G698" s="18"/>
     </row>
-    <row r="699" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="699" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G699" s="18"/>
     </row>
-    <row r="700" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="700" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G700" s="18"/>
     </row>
-    <row r="701" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="701" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G701" s="18"/>
     </row>
-    <row r="702" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="702" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G702" s="18"/>
     </row>
-    <row r="703" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="703" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G703" s="18"/>
     </row>
-    <row r="704" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="704" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G704" s="18"/>
     </row>
-    <row r="705" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="705" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G705" s="18"/>
     </row>
-    <row r="706" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="706" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G706" s="18"/>
     </row>
-    <row r="707" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="707" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G707" s="18"/>
     </row>
-    <row r="708" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="708" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G708" s="18"/>
     </row>
-    <row r="709" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="709" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G709" s="18"/>
     </row>
-    <row r="710" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="710" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G710" s="18"/>
     </row>
-    <row r="711" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="711" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G711" s="18"/>
     </row>
-    <row r="712" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="712" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G712" s="18"/>
     </row>
-    <row r="713" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="713" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G713" s="18"/>
     </row>
-    <row r="714" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="714" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G714" s="18"/>
     </row>
-    <row r="715" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="715" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G715" s="18"/>
     </row>
-    <row r="716" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="716" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G716" s="18"/>
     </row>
-    <row r="717" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="717" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G717" s="18"/>
     </row>
-    <row r="718" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="718" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G718" s="18"/>
     </row>
-    <row r="719" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="719" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G719" s="18"/>
     </row>
-    <row r="720" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="720" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G720" s="18"/>
     </row>
-    <row r="721" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="721" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G721" s="18"/>
     </row>
-    <row r="722" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="722" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G722" s="18"/>
     </row>
-    <row r="723" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="723" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G723" s="18"/>
     </row>
-    <row r="724" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="724" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G724" s="18"/>
     </row>
-    <row r="725" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="725" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G725" s="18"/>
     </row>
-    <row r="726" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="726" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G726" s="18"/>
     </row>
-    <row r="727" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="727" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G727" s="18"/>
     </row>
-    <row r="728" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="728" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G728" s="18"/>
     </row>
-    <row r="729" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="729" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G729" s="18"/>
     </row>
-    <row r="730" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="730" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G730" s="18"/>
     </row>
-    <row r="731" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="731" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G731" s="18"/>
     </row>
-    <row r="732" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="732" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G732" s="18"/>
     </row>
-    <row r="733" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="733" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G733" s="18"/>
     </row>
-    <row r="734" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="734" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G734" s="18"/>
     </row>
-    <row r="735" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="735" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G735" s="18"/>
     </row>
-    <row r="736" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="736" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G736" s="18"/>
     </row>
-    <row r="737" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="737" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G737" s="18"/>
     </row>
-    <row r="738" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="738" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G738" s="18"/>
     </row>
-    <row r="739" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="739" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G739" s="18"/>
     </row>
-    <row r="740" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="740" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G740" s="18"/>
     </row>
-    <row r="741" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="741" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G741" s="18"/>
     </row>
-    <row r="742" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="742" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G742" s="18"/>
     </row>
-    <row r="743" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="743" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G743" s="18"/>
     </row>
-    <row r="744" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="744" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G744" s="18"/>
     </row>
-    <row r="745" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="745" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G745" s="18"/>
     </row>
-    <row r="746" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="746" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G746" s="18"/>
     </row>
-    <row r="747" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="747" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G747" s="18"/>
     </row>
-    <row r="748" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="748" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G748" s="18"/>
     </row>
-    <row r="749" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="749" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G749" s="18"/>
     </row>
-    <row r="750" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="750" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G750" s="18"/>
     </row>
-    <row r="751" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="751" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G751" s="18"/>
     </row>
-    <row r="752" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="752" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G752" s="18"/>
     </row>
-    <row r="753" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="753" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G753" s="18"/>
     </row>
-    <row r="754" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="754" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G754" s="18"/>
     </row>
-    <row r="755" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="755" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G755" s="18"/>
     </row>
-    <row r="756" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="756" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G756" s="18"/>
     </row>
-    <row r="757" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="757" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G757" s="18"/>
     </row>
-    <row r="758" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="758" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G758" s="18"/>
     </row>
-    <row r="759" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="759" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G759" s="18"/>
     </row>
-    <row r="760" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="760" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G760" s="18"/>
     </row>
-    <row r="761" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="761" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G761" s="18"/>
     </row>
-    <row r="762" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="762" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G762" s="18"/>
     </row>
-    <row r="763" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="763" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G763" s="18"/>
     </row>
-    <row r="764" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="764" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G764" s="18"/>
     </row>
-    <row r="765" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="765" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G765" s="18"/>
     </row>
-    <row r="766" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="766" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G766" s="18"/>
     </row>
-    <row r="767" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="767" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G767" s="18"/>
     </row>
-    <row r="768" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="768" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G768" s="18"/>
     </row>
-    <row r="769" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="769" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G769" s="18"/>
     </row>
-    <row r="770" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="770" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G770" s="18"/>
     </row>
-    <row r="771" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="771" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G771" s="18"/>
     </row>
-    <row r="772" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="772" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G772" s="18"/>
     </row>
-    <row r="773" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="773" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G773" s="18"/>
     </row>
-    <row r="774" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="774" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G774" s="18"/>
     </row>
-    <row r="775" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="775" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G775" s="18"/>
     </row>
-    <row r="776" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="776" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G776" s="18"/>
     </row>
-    <row r="777" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="777" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G777" s="18"/>
     </row>
-    <row r="778" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="778" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G778" s="18"/>
     </row>
-    <row r="779" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="779" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G779" s="18"/>
     </row>
-    <row r="780" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="780" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G780" s="18"/>
     </row>
-    <row r="781" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="781" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G781" s="18"/>
     </row>
-    <row r="782" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="782" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G782" s="18"/>
     </row>
-    <row r="783" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="783" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G783" s="18"/>
     </row>
-    <row r="784" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="784" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G784" s="18"/>
     </row>
-    <row r="785" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="785" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G785" s="18"/>
     </row>
-    <row r="786" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="786" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G786" s="18"/>
     </row>
-    <row r="787" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="787" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G787" s="18"/>
     </row>
-    <row r="788" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="788" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G788" s="18"/>
     </row>
-    <row r="789" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="789" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G789" s="18"/>
     </row>
-    <row r="790" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="790" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G790" s="18"/>
     </row>
-    <row r="791" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="791" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G791" s="18"/>
     </row>
-    <row r="792" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="792" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G792" s="18"/>
     </row>
-    <row r="793" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="793" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G793" s="18"/>
     </row>
-    <row r="794" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="794" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G794" s="18"/>
     </row>
-    <row r="795" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="795" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G795" s="18"/>
     </row>
-    <row r="796" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="796" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G796" s="18"/>
     </row>
-    <row r="797" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="797" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G797" s="18"/>
     </row>
-    <row r="798" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="798" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G798" s="18"/>
     </row>
-    <row r="799" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="799" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G799" s="18"/>
     </row>
-    <row r="800" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="800" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G800" s="18"/>
     </row>
-    <row r="801" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="801" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G801" s="18"/>
     </row>
-    <row r="802" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="802" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G802" s="18"/>
     </row>
-    <row r="803" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="803" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G803" s="18"/>
     </row>
-    <row r="804" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="804" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G804" s="18"/>
     </row>
-    <row r="805" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="805" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G805" s="18"/>
     </row>
-    <row r="806" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="806" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G806" s="18"/>
     </row>
-    <row r="807" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="807" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G807" s="18"/>
     </row>
-    <row r="808" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="808" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G808" s="18"/>
     </row>
-    <row r="809" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="809" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G809" s="18"/>
     </row>
-    <row r="810" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="810" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G810" s="18"/>
     </row>
-    <row r="811" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="811" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G811" s="18"/>
     </row>
-    <row r="812" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="812" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G812" s="18"/>
     </row>
-    <row r="813" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="813" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G813" s="18"/>
     </row>
-    <row r="814" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="814" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G814" s="18"/>
     </row>
-    <row r="815" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="815" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G815" s="18"/>
     </row>
-    <row r="816" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="816" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G816" s="18"/>
     </row>
-    <row r="817" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="817" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G817" s="18"/>
     </row>
-    <row r="818" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="818" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G818" s="18"/>
     </row>
-    <row r="819" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="819" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G819" s="18"/>
     </row>
-    <row r="820" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="820" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G820" s="18"/>
     </row>
-    <row r="821" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="821" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G821" s="18"/>
     </row>
-    <row r="822" spans="7:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="822" spans="7:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G822" s="18"/>
     </row>
   </sheetData>
@@ -4141,17 +4186,17 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <f>COUNTA(NOTICE!D2:D17)</f>
         <v>3</v>

</xml_diff>